<commit_message>
New Org Production Debugging
</commit_message>
<xml_diff>
--- a/TestData/Production/Web_POS/Billing/add_to_cart_test_data.xlsx
+++ b/TestData/Production/Web_POS/Billing/add_to_cart_test_data.xlsx
@@ -105,7 +105,7 @@
     <t>TC_02</t>
   </si>
   <si>
-    <t>Alexa67 : 1</t>
+    <t>Alexa678 : 1</t>
   </si>
   <si>
     <t>TC_03</t>
@@ -138,37 +138,37 @@
     <t>TC_28</t>
   </si>
   <si>
-    <t>Alexa67 : 1.8</t>
+    <t>Alexa678 : 1.8</t>
   </si>
   <si>
     <t>TC_29</t>
   </si>
   <si>
-    <t>Alexa67 : 1.9</t>
+    <t>Alexa678 : 1.9</t>
   </si>
   <si>
     <t>TC_30</t>
   </si>
   <si>
-    <t>Alexa67 : 1.10</t>
+    <t>Alexa678 : 1.10</t>
   </si>
   <si>
     <t>TC_31</t>
   </si>
   <si>
-    <t>Alexa67 : 1.11</t>
+    <t>Alexa678 : 1.11</t>
   </si>
   <si>
     <t>TC_32</t>
   </si>
   <si>
-    <t>Alexa67 : 1.12</t>
+    <t>Alexa678 : 1.12</t>
   </si>
   <si>
     <t>TC_33</t>
   </si>
   <si>
-    <t>Alexa67 : 1.13</t>
+    <t>Alexa678 : 1.13</t>
   </si>
   <si>
     <t>TC_34</t>
@@ -225,25 +225,8 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border/>
-    <border>
-      <left>
-        <color indexed="64"/>
-      </left>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top>
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-      <diagonal>
-        <color indexed="64"/>
-      </diagonal>
-    </border>
     <border>
       <right style="medium">
         <color rgb="FF2B579A"/>
@@ -256,21 +239,19 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -492,7 +473,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="I1">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
@@ -511,7 +492,7 @@
     <col min="13" max="13" width="10.71094" customWidth="1"/>
     <col min="14" max="14" width="10.71094" customWidth="1"/>
     <col min="15" max="15" width="19.14063" customWidth="1"/>
-    <col min="16" max="16" width="24.48047" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.48047" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="36.25" style="1" customWidth="1"/>
     <col min="18" max="18" width="22.5" style="1" customWidth="1"/>
     <col min="19" max="19" width="22.5" style="1" customWidth="1"/>
@@ -528,19 +509,19 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -570,7 +551,7 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -578,19 +559,19 @@
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>1234</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>123456</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -605,19 +586,19 @@
       <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="3">
         <v>45384</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2">
         <v>3636363636</v>
       </c>
     </row>
@@ -625,19 +606,19 @@
       <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1234</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>123456</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -652,19 +633,19 @@
       <c r="J3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>45384</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3">
         <v>3636363636</v>
       </c>
     </row>
@@ -672,19 +653,19 @@
       <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>1234</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>123456</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -699,19 +680,19 @@
       <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>45384</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4">
         <v>3636363636</v>
       </c>
     </row>
@@ -719,19 +700,19 @@
       <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>1234</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>123456</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -746,19 +727,19 @@
       <c r="J5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>45384</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5">
         <v>3636363636</v>
       </c>
     </row>
@@ -766,19 +747,19 @@
       <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>1234</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>123456</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -793,19 +774,19 @@
       <c r="J6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <v>45384</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="2">
         <v>9874563211</v>
       </c>
     </row>
@@ -813,19 +794,19 @@
       <c r="A7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>1234</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>123456</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -840,19 +821,19 @@
       <c r="J7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>45384</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7">
         <v>3636363636</v>
       </c>
     </row>
@@ -860,19 +841,19 @@
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>1234</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>123456</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -887,19 +868,19 @@
       <c r="J8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <v>45384</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="2">
         <v>9874563211</v>
       </c>
     </row>
@@ -907,19 +888,19 @@
       <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>1234</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>123456</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -934,19 +915,19 @@
       <c r="J9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="3">
         <v>45384</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9">
         <v>3636363636</v>
       </c>
     </row>
@@ -954,19 +935,19 @@
       <c r="A10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>1234</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>123456</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -981,19 +962,19 @@
       <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <v>45384</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="N10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P10" s="5">
+      <c r="P10" s="2">
         <v>9874563211</v>
       </c>
     </row>
@@ -1001,19 +982,19 @@
       <c r="A11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>1234</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>123456</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1028,19 +1009,19 @@
       <c r="J11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <v>45384</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11">
         <v>3636363636</v>
       </c>
     </row>
@@ -1048,19 +1029,19 @@
       <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>1234</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>123456</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1075,19 +1056,19 @@
       <c r="J12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="3">
         <v>45384</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="N12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12">
         <v>3636363636</v>
       </c>
     </row>
@@ -1095,19 +1076,19 @@
       <c r="A13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>1234</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>123456</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1122,19 +1103,19 @@
       <c r="J13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="3">
         <v>45384</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="N13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13">
         <v>3636363636</v>
       </c>
     </row>
@@ -1142,19 +1123,19 @@
       <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>1234</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>123456</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -1169,19 +1150,19 @@
       <c r="J14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="3">
         <v>45384</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="N14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="5">
+      <c r="P14" s="2">
         <v>9874563211</v>
       </c>
     </row>
@@ -1189,19 +1170,19 @@
       <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>1234</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>123456</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1216,19 +1197,19 @@
       <c r="J15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="3">
         <v>45384</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="N15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15">
         <v>3636363636</v>
       </c>
     </row>
@@ -1236,19 +1217,19 @@
       <c r="A16" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>1234</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>123456</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1263,19 +1244,19 @@
       <c r="J16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="3">
         <v>45384</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="N16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P16" s="5">
+      <c r="P16" s="2">
         <v>9874563211</v>
       </c>
     </row>
@@ -1283,19 +1264,19 @@
       <c r="A17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>1234</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>123456</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -1310,19 +1291,19 @@
       <c r="J17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="3">
         <v>45384</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="N17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17">
         <v>3636363636</v>
       </c>
     </row>
@@ -1330,19 +1311,19 @@
       <c r="A18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>1234</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>123456</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -1357,19 +1338,19 @@
       <c r="J18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="3">
         <v>45384</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="N18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P18">
         <v>3636363636</v>
       </c>
     </row>
@@ -1377,19 +1358,19 @@
       <c r="A19" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>1234</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>123456</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -1404,163 +1385,163 @@
       <c r="J19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="3">
         <v>45384</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N19" s="4" t="s">
+      <c r="N19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P19">
         <v>3636363636</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="P20" s="5"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="P20" s="2"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="P21" s="5"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="P21" s="2"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="P22" s="5"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="P22" s="2"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="P23" s="5"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="P23" s="2"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="7"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="5"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="P25" s="5"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="P25" s="2"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="P26" s="5"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="P26" s="2"/>
     </row>
     <row r="27" ht="14.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="P27" s="5"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="P27" s="2"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="P28" s="5"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="P28" s="2"/>
     </row>
     <row r="29" ht="12.75">
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="7"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="5"/>
     </row>
     <row r="30" ht="12.75">
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="7"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="5"/>
     </row>
     <row r="31" ht="12.75">
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="7"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="5"/>
     </row>
     <row r="32" ht="12.75">
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="6"/>
-      <c r="T32" s="7"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="5"/>
     </row>
     <row r="33" ht="12.75">
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="7"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="5"/>
     </row>
     <row r="34" ht="12.75">
       <c r="T34" s="1"/>
@@ -1569,371 +1550,371 @@
       <c r="T35" s="1"/>
     </row>
     <row r="36" ht="12.75">
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="7"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="5"/>
     </row>
     <row r="38" ht="14.25">
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
       <c r="J38" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="6"/>
-      <c r="T38" s="7"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="5"/>
     </row>
     <row r="39" ht="14.25">
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
       <c r="J39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="P39" s="5"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="P39" s="2"/>
     </row>
     <row r="40" ht="14.25">
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
       <c r="J40" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="P40" s="5"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="P40" s="2"/>
     </row>
     <row r="41" ht="14.25">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
       <c r="J41" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="P41" s="5"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="P41" s="2"/>
     </row>
     <row r="42" ht="14.25">
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
       <c r="J42" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="P42" s="5"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="P42" s="2"/>
     </row>
     <row r="43" ht="14.25">
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
       <c r="J43" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="P43" s="5"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="P43" s="2"/>
     </row>
     <row r="44" ht="14.25">
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
       <c r="J44" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="P44" s="5"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="P44" s="2"/>
     </row>
     <row r="45" ht="14.25">
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
       <c r="J45" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="P45" s="5"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="P45" s="2"/>
     </row>
     <row r="46" ht="14.25">
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
       <c r="J46" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="P46" s="5"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="P46" s="2"/>
     </row>
     <row r="47" ht="14.25">
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
       <c r="J47" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="P47" s="5"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="P47" s="2"/>
     </row>
     <row r="48" ht="14.25">
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="P48" s="5"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="P48" s="2"/>
     </row>
     <row r="49" ht="14.25">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
       <c r="J49" s="1"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="P49" s="5"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="P49" s="2"/>
     </row>
     <row r="50" ht="14.25">
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
       <c r="J50" s="1"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="P50" s="5"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="P50" s="2"/>
     </row>
     <row r="51" ht="14.25">
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="P51" s="5"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="P51" s="2"/>
     </row>
     <row r="52" ht="14.25">
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
       <c r="J52" s="1"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
-      <c r="N52" s="4"/>
-      <c r="P52" s="5"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="P52" s="2"/>
     </row>
     <row r="53" ht="14.25">
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
       <c r="J53" s="1"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="P53" s="5"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="P53" s="2"/>
     </row>
     <row r="54" ht="14.25">
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
       <c r="J54" s="1"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="P54" s="5"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="P54" s="2"/>
     </row>
     <row r="55" ht="14.25">
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
       <c r="J55" s="1"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="P55" s="5"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="P55" s="2"/>
     </row>
     <row r="56" ht="14.25">
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
-      <c r="P56" s="5"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="P56" s="2"/>
     </row>
     <row r="57" ht="14.25">
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="4"/>
-      <c r="P57" s="5"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="P57" s="2"/>
     </row>
     <row r="58" ht="14.25">
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-      <c r="P58" s="5"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="P58" s="2"/>
     </row>
     <row r="59" ht="14.25">
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="P59" s="5"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="P59" s="2"/>
     </row>
     <row r="60" ht="14.25">
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="P60" s="5"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="P60" s="2"/>
     </row>
     <row r="61" ht="14.25">
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
       <c r="J61" s="1"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="P61" s="5"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="P61" s="2"/>
     </row>
     <row r="62" ht="14.25">
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
       <c r="J62" s="1"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
-      <c r="N62" s="4"/>
-      <c r="P62" s="5"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="P62" s="2"/>
     </row>
     <row r="63" ht="14.25">
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
       <c r="J63" s="1"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="P63" s="5"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="P63" s="2"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="I64"/>

</xml_diff>